<commit_message>
ửa lỗi bị ghi đè ở biểu đồ so sánh thời gian
</commit_message>
<xml_diff>
--- a/KetQuaThucNghiem.xlsx
+++ b/KetQuaThucNghiem.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\THUC TAP CO SO NGANH\CODE\GA_Baitoancaitui_OOP_22-11-2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\THUC TAP CO SO NGANH\CODE\GA_Baitoancaitui_OOP_Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1802F4-5024-4126-83CE-450E3507B71D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17F877F-8760-4660-9F4D-26F633A1635C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -452,7 +452,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Sử lỗi golic chạy và khoởi tạo
</commit_message>
<xml_diff>
--- a/KetQuaThucNghiem.xlsx
+++ b/KetQuaThucNghiem.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\THUC TAP CO SO NGANH\CODE\GA_Baitoancaitui_OOP_Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17F877F-8760-4660-9F4D-26F633A1635C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3F8295-A217-4F73-808E-DAE37E43B52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4030" yWindow="3040" windowWidth="17270" windowHeight="9820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kết quả thực nghiệm" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="22">
   <si>
     <t>Bộ dữ liệu</t>
   </si>
@@ -62,12 +62,37 @@
   </si>
   <si>
     <t>10.10item</t>
+  </si>
+  <si>
+    <t>NgauNhien_n10_W20</t>
+  </si>
+  <si>
+    <t>24item</t>
+  </si>
+  <si>
+    <t>200item</t>
+  </si>
+  <si>
+    <t>500item</t>
+  </si>
+  <si>
+    <t>15item</t>
+  </si>
+  <si>
+    <t>50item</t>
+  </si>
+  <si>
+    <t>100item</t>
+  </si>
+  <si>
+    <t>NgauNhien_n4_W20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -120,8 +145,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A4E802BE-F88E-494D-A842-F162421CC05B}" name="Table1" displayName="Table1" ref="A1:D11" totalsRowShown="0">
-  <autoFilter ref="A1:D11" xr:uid="{A4E802BE-F88E-494D-A842-F162421CC05B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A4E802BE-F88E-494D-A842-F162421CC05B}" name="Table1" displayName="Table1" ref="A1:D12" totalsRowShown="0">
+  <autoFilter ref="A1:D12" xr:uid="{A4E802BE-F88E-494D-A842-F162421CC05B}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{04C68727-00FC-4FEF-8A93-D2C4334301B3}" name="Bộ dữ liệu"/>
     <tableColumn id="2" xr3:uid="{97C4DB5B-5C3F-4B34-AE0A-7B79E5221371}" name="Fitness tối ưu"/>
@@ -449,7 +474,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
@@ -457,14 +482,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.453125" customWidth="1"/>
-    <col min="2" max="2" width="14.08984375" customWidth="1"/>
-    <col min="3" max="3" width="18.90625" customWidth="1"/>
-    <col min="4" max="4" width="16.26953125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.453125"/>
+    <col min="2" max="2" customWidth="true" width="14.08984375"/>
+    <col min="3" max="3" customWidth="true" width="18.90625"/>
+    <col min="4" max="4" customWidth="true" width="16.26953125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -478,143 +503,801 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0">
         <v>309</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>1392</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>1158</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="0">
         <v>149</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="0">
         <v>1441</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>1225</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="0">
         <v>266</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="0">
         <v>1249</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <v>1076</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="0">
         <v>261</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="0">
         <v>1406</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="0">
         <v>1200</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="0">
         <v>332</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="0">
         <v>1246</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="0">
         <v>1091</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="0">
         <v>148</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="0">
         <v>1148</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="0">
         <v>1159</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="0">
         <v>308</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="0">
         <v>1146</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="0">
         <v>1030</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="0">
         <v>322</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="0">
         <v>1131</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="0">
         <v>1117</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="0">
         <v>333</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="0">
         <v>1105</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="0">
         <v>1101</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="0">
         <v>339</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="0">
         <v>1060</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="0">
         <v>1002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B12" s="0">
+        <v>339</v>
+      </c>
+      <c r="C12" s="0">
+        <v>1716</v>
+      </c>
+      <c r="D12" s="0">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B13" t="n" s="0">
+        <v>55.0</v>
+      </c>
+      <c r="C13" t="n" s="0">
+        <v>1306.0</v>
+      </c>
+      <c r="D13" t="n" s="0">
+        <v>1004.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B14" t="n" s="0">
+        <v>38.0</v>
+      </c>
+      <c r="C14" t="n" s="0">
+        <v>679.0</v>
+      </c>
+      <c r="D14" t="n" s="0">
+        <v>260.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B15" t="n" s="0">
+        <v>1.3297089E7</v>
+      </c>
+      <c r="C15" t="n" s="0">
+        <v>1121.0</v>
+      </c>
+      <c r="D15" t="n" s="0">
+        <v>204.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B16" t="n" s="0">
+        <v>-9.9904101E7</v>
+      </c>
+      <c r="C16" t="n" s="0">
+        <v>25344.0</v>
+      </c>
+      <c r="D16" t="n" s="0">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B17" t="n" s="0">
+        <v>-9.9990593E8</v>
+      </c>
+      <c r="C17" t="n" s="0">
+        <v>15624.0</v>
+      </c>
+      <c r="D17" t="n" s="0">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n" s="0">
+        <v>87632.0</v>
+      </c>
+      <c r="C18" t="n" s="0">
+        <v>31490.0</v>
+      </c>
+      <c r="D18" t="n" s="0">
+        <v>205.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B19" t="n" s="0">
+        <v>2.4437641E7</v>
+      </c>
+      <c r="C19" t="n" s="0">
+        <v>691.0</v>
+      </c>
+      <c r="D19" t="n" s="0">
+        <v>137.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B20" t="n" s="0">
+        <v>1.3228166E7</v>
+      </c>
+      <c r="C20" t="n" s="0">
+        <v>835.0</v>
+      </c>
+      <c r="D20" t="n" s="0">
+        <v>128.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B21" t="n" s="0">
+        <v>2.145685493E9</v>
+      </c>
+      <c r="C21" t="n" s="0">
+        <v>820.0</v>
+      </c>
+      <c r="D21" t="n" s="0">
+        <v>122.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B22" t="n" s="0">
+        <v>2.144986177E9</v>
+      </c>
+      <c r="C22" t="n" s="0">
+        <v>792.0</v>
+      </c>
+      <c r="D22" t="n" s="0">
+        <v>117.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B23" t="n" s="0">
+        <v>2.14740958E9</v>
+      </c>
+      <c r="C23" t="n" s="0">
+        <v>1102.0</v>
+      </c>
+      <c r="D23" t="n" s="0">
+        <v>234.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B24" t="n" s="0">
+        <v>2.146159776E9</v>
+      </c>
+      <c r="C24" t="n" s="0">
+        <v>1398.0</v>
+      </c>
+      <c r="D24" t="n" s="0">
+        <v>343.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B25" t="n" s="0">
+        <v>1.3371989E7</v>
+      </c>
+      <c r="C25" t="n" s="0">
+        <v>897.0</v>
+      </c>
+      <c r="D25" t="n" s="0">
+        <v>149.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B26" t="n" s="0">
+        <v>-2993696.0</v>
+      </c>
+      <c r="C26" t="n" s="0">
+        <v>25653.0</v>
+      </c>
+      <c r="D26" t="n" s="0">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B27" t="n" s="0">
+        <v>1.3404517E7</v>
+      </c>
+      <c r="C27" t="n" s="0">
+        <v>850.0</v>
+      </c>
+      <c r="D27" t="n" s="0">
+        <v>137.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="C28" t="n" s="0">
+        <v>24435.0</v>
+      </c>
+      <c r="D28" t="n" s="0">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B29" t="n" s="0">
+        <v>1.3238481E7</v>
+      </c>
+      <c r="C29" t="n" s="0">
+        <v>1166.0</v>
+      </c>
+      <c r="D29" t="n" s="0">
+        <v>262.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B30" t="n" s="0">
+        <v>-9.9904026E7</v>
+      </c>
+      <c r="C30" t="n" s="0">
+        <v>24808.0</v>
+      </c>
+      <c r="D30" t="n" s="0">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B31" t="n" s="0">
+        <v>1.3351011E7</v>
+      </c>
+      <c r="C31" t="n" s="0">
+        <v>1280.0</v>
+      </c>
+      <c r="D31" t="n" s="0">
+        <v>297.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B32" t="n" s="0">
+        <v>-9.9905318E7</v>
+      </c>
+      <c r="C32" t="n" s="0">
+        <v>25649.0</v>
+      </c>
+      <c r="D32" t="n" s="0">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B33" t="n" s="0">
+        <v>1.3273034E7</v>
+      </c>
+      <c r="C33" t="n" s="0">
+        <v>761.0</v>
+      </c>
+      <c r="D33" t="n" s="0">
+        <v>101.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B34" t="n" s="0">
+        <v>3298.0</v>
+      </c>
+      <c r="C34" t="n" s="0">
+        <v>24874.0</v>
+      </c>
+      <c r="D34" t="n" s="0">
+        <v>101.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B35" t="n" s="0">
+        <v>309.0</v>
+      </c>
+      <c r="C35" t="n" s="0">
+        <v>551.0</v>
+      </c>
+      <c r="D35" t="n" s="0">
+        <v>101.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B36" t="n" s="0">
+        <v>1.3412889E7</v>
+      </c>
+      <c r="C36" t="n" s="0">
+        <v>898.0</v>
+      </c>
+      <c r="D36" t="n" s="0">
+        <v>166.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B37" t="n" s="0">
+        <v>3592.0</v>
+      </c>
+      <c r="C37" t="n" s="0">
+        <v>24491.0</v>
+      </c>
+      <c r="D37" t="n" s="0">
+        <v>101.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B38" t="n" s="0">
+        <v>1450.0</v>
+      </c>
+      <c r="C38" t="n" s="0">
+        <v>150427.0</v>
+      </c>
+      <c r="D38" t="n" s="0">
+        <v>101.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B39" t="n" s="0">
+        <v>309.0</v>
+      </c>
+      <c r="C39" t="n" s="0">
+        <v>262.0</v>
+      </c>
+      <c r="D39" t="n" s="0">
+        <v>257.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B40" t="n" s="0">
+        <v>1.3491239E7</v>
+      </c>
+      <c r="C40" t="n" s="0">
+        <v>1105.0</v>
+      </c>
+      <c r="D40" t="n" s="0">
+        <v>213.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B41" t="n" s="0">
+        <v>1340.0</v>
+      </c>
+      <c r="C41" t="n" s="0">
+        <v>154626.0</v>
+      </c>
+      <c r="D41" t="n" s="0">
+        <v>101.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B42" t="n" s="0">
+        <v>3160.0</v>
+      </c>
+      <c r="C42" t="n" s="0">
+        <v>24881.0</v>
+      </c>
+      <c r="D42" t="n" s="0">
+        <v>101.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B43" t="n" s="0">
+        <v>1446.0</v>
+      </c>
+      <c r="C43" t="n" s="0">
+        <v>369.0</v>
+      </c>
+      <c r="D43" t="n" s="0">
+        <v>169.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B44" t="n" s="0">
+        <v>2086.0</v>
+      </c>
+      <c r="C44" t="n" s="0">
+        <v>2535.0</v>
+      </c>
+      <c r="D44" t="n" s="0">
+        <v>202.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B45" t="n" s="0">
+        <v>5949.0</v>
+      </c>
+      <c r="C45" t="n" s="0">
+        <v>15597.0</v>
+      </c>
+      <c r="D45" t="n" s="0">
+        <v>101.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B46" t="n" s="0">
+        <v>4163.0</v>
+      </c>
+      <c r="C46" t="n" s="0">
+        <v>6724.0</v>
+      </c>
+      <c r="D46" t="n" s="0">
+        <v>163.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B47" t="n" s="0">
+        <v>2082.0</v>
+      </c>
+      <c r="C47" t="n" s="0">
+        <v>6430.0</v>
+      </c>
+      <c r="D47" t="n" s="0">
+        <v>395.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B48" t="n" s="0">
+        <v>4137.0</v>
+      </c>
+      <c r="C48" t="n" s="0">
+        <v>10630.0</v>
+      </c>
+      <c r="D48" t="n" s="0">
+        <v>172.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B49" t="n" s="0">
+        <v>4381.0</v>
+      </c>
+      <c r="C49" t="n" s="0">
+        <v>53055.0</v>
+      </c>
+      <c r="D49" t="n" s="0">
+        <v>1388.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B50" t="n" s="0">
+        <v>5482.0</v>
+      </c>
+      <c r="C50" t="n" s="0">
+        <v>78551.0</v>
+      </c>
+      <c r="D50" t="n" s="0">
+        <v>2075.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B51" t="n" s="0">
+        <v>2109.0</v>
+      </c>
+      <c r="C51" t="n" s="0">
+        <v>32514.0</v>
+      </c>
+      <c r="D51" t="n" s="0">
+        <v>2042.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B52" t="n" s="0">
+        <v>16289.0</v>
+      </c>
+      <c r="C52" t="n" s="0">
+        <v>247053.0</v>
+      </c>
+      <c r="D52" t="n" s="0">
+        <v>1001.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B53" t="n" s="0">
+        <v>31.0</v>
+      </c>
+      <c r="C53" t="n" s="0">
+        <v>1256.0</v>
+      </c>
+      <c r="D53" t="n" s="0">
+        <v>1001.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B54" t="n" s="0">
+        <v>2113.0</v>
+      </c>
+      <c r="C54" t="n" s="0">
+        <v>32235.0</v>
+      </c>
+      <c r="D54" t="n" s="0">
+        <v>1839.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B55" t="n" s="0">
+        <v>219.0</v>
+      </c>
+      <c r="C55" t="n" s="0">
+        <v>1380.0</v>
+      </c>
+      <c r="D55" t="n" s="0">
+        <v>1007.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B56" t="n" s="0">
+        <v>1.3121473E7</v>
+      </c>
+      <c r="C56" t="n" s="0">
+        <v>4007.0</v>
+      </c>
+      <c r="D56" t="n" s="0">
+        <v>1007.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B57" t="n" s="0">
+        <v>1.3239574E7</v>
+      </c>
+      <c r="C57" t="n" s="0">
+        <v>3042.0</v>
+      </c>
+      <c r="D57" t="n" s="0">
+        <v>1024.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B58" t="n" s="0">
+        <v>419.0</v>
+      </c>
+      <c r="C58" t="n" s="0">
+        <v>6360.0</v>
+      </c>
+      <c r="D58" t="n" s="0">
+        <v>2420.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>